<commit_message>
Compute X Interpolants once.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA875D5-0EDB-4039-86EB-5D7490C62192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730F62B0-0395-4221-B2CB-65688F80AB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tex, Flags&lt;0&gt;" sheetId="1" r:id="rId1"/>
+    <sheet name="Flat, Flags&lt;0&gt;" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>GCC Win</t>
   </si>
@@ -38,11 +39,20 @@
   <si>
     <t>Baseline</t>
   </si>
+  <si>
+    <t>X Delta once</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,19 +399,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19275CA-BC63-49E0-893C-9314B492270F}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +423,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -424,6 +440,72 @@
       <c r="D2">
         <v>56</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>71957</v>
+      </c>
+      <c r="C3">
+        <v>73067</v>
+      </c>
+      <c r="D3">
+        <v>76</v>
+      </c>
+      <c r="E3" s="1">
+        <f>(D3/D2)-1</f>
+        <v>0.35714285714285721</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0AC41-34A4-4C4B-992F-CC4F79B64425}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>155448</v>
+      </c>
+      <c r="C2">
+        <v>165920</v>
+      </c>
+      <c r="D2">
+        <v>396</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Vertex order as ints.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5042321-E16A-408B-A850-419F79C1EB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1AEC9A-72B1-4AC4-B70E-7294057956D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>GCC Win</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Preload color</t>
+  </si>
+  <si>
+    <t>Order int</t>
+  </si>
+  <si>
+    <t>Order</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19275CA-BC63-49E0-893C-9314B492270F}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +591,7 @@
         <v>75</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" ref="E6:E12" si="2">(D6/D$2)-1</f>
+        <f t="shared" ref="E6:E13" si="2">(D6/D$2)-1</f>
         <v>0.33928571428571419</v>
       </c>
       <c r="F6" s="1">
@@ -729,6 +735,18 @@
       <c r="F12" s="1">
         <f t="shared" si="1"/>
         <v>6.5217391304347894E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>98</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>
@@ -739,10 +757,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0AC41-34A4-4C4B-992F-CC4F79B64425}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,6 +884,22 @@
         <v>3.1152647975077885E-2</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>332</v>
+      </c>
+      <c r="E7" s="1">
+        <f>(D7/D$2)-1</f>
+        <v>-0.16161616161616166</v>
+      </c>
+      <c r="F7" s="1">
+        <f>(D7/D6)-1</f>
+        <v>3.0211480362538623E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -876,7 +910,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,11 +997,11 @@
         <v>161733</v>
       </c>
       <c r="D6">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E6" s="1">
         <f>(D6/D$2)-1</f>
-        <v>2.3775510204081631</v>
+        <v>2.3877551020408165</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -990,7 +1024,7 @@
       </c>
       <c r="F7" s="1">
         <f>(D7/D6)-1</f>
-        <v>-0.11178247734138969</v>
+        <v>-0.11445783132530118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sort vertexes without copy.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA86D444-1910-4953-AADC-4C4BFF8F407F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E101C00F-6172-4851-8034-8130EF2619D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>GCC Win</t>
   </si>
@@ -137,6 +137,18 @@
   </si>
   <si>
     <t>Guard band clip frustrum</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Refactor</t>
+  </si>
+  <si>
+    <t>IWRAM</t>
+  </si>
+  <si>
+    <t>In place sort</t>
   </si>
 </sst>
 </file>
@@ -492,10 +504,465 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19275CA-BC63-49E0-893C-9314B492270F}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>53163</v>
+      </c>
+      <c r="C2">
+        <v>55959</v>
+      </c>
+      <c r="D2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>71957</v>
+      </c>
+      <c r="C3">
+        <v>73067</v>
+      </c>
+      <c r="D3">
+        <v>76</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E5" si="0">(D3/D$2)-1</f>
+        <v>0.35714285714285721</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F18" si="1">(D3/D2)-1</f>
+        <v>0.35714285714285721</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>71797</v>
+      </c>
+      <c r="C4">
+        <v>72327</v>
+      </c>
+      <c r="D4">
+        <v>75</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33928571428571419</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.3157894736842146E-2</v>
+      </c>
+      <c r="H4">
+        <v>16868</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>59326</v>
+      </c>
+      <c r="C5">
+        <v>69900</v>
+      </c>
+      <c r="D5">
+        <v>75</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33928571428571419</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>17968</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>72364</v>
+      </c>
+      <c r="C6">
+        <v>72280</v>
+      </c>
+      <c r="D6">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" ref="E6:E14" si="2">(D6/D$2)-1</f>
+        <v>0.33928571428571419</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>17780</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>77875</v>
+      </c>
+      <c r="C7">
+        <v>76905</v>
+      </c>
+      <c r="D7">
+        <v>84</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.12000000000000011</v>
+      </c>
+      <c r="H7">
+        <v>17324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>77435</v>
+      </c>
+      <c r="C8">
+        <v>78173</v>
+      </c>
+      <c r="D8">
+        <v>83</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>0.48214285714285721</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.1904761904761862E-2</v>
+      </c>
+      <c r="H8">
+        <v>16972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>78045</v>
+      </c>
+      <c r="C9">
+        <v>69808</v>
+      </c>
+      <c r="D9">
+        <v>88</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>6.024096385542177E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>78585</v>
+      </c>
+      <c r="C10">
+        <v>70771</v>
+      </c>
+      <c r="D10">
+        <v>90</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60714285714285721</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2727272727272707E-2</v>
+      </c>
+      <c r="H10">
+        <v>16928</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>92</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.64285714285714279</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2222222222222143E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>82020</v>
+      </c>
+      <c r="C12">
+        <v>72108</v>
+      </c>
+      <c r="D12">
+        <v>98</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>6.5217391304347894E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>82169</v>
+      </c>
+      <c r="C13">
+        <v>73632</v>
+      </c>
+      <c r="D13">
+        <v>98</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>16908</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14">
+        <v>79126</v>
+      </c>
+      <c r="C14">
+        <v>65203</v>
+      </c>
+      <c r="D14">
+        <v>99</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.76785714285714279</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0204081632652962E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
+        <v>98483</v>
+      </c>
+      <c r="C15">
+        <v>90661</v>
+      </c>
+      <c r="D15">
+        <v>115</v>
+      </c>
+      <c r="E15" s="1">
+        <f>(D15/D$2)-1</f>
+        <v>1.0535714285714284</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.16161616161616155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>98921</v>
+      </c>
+      <c r="C16">
+        <v>89968</v>
+      </c>
+      <c r="D16">
+        <v>114</v>
+      </c>
+      <c r="E16" s="1">
+        <f>(D16/D$2)-1</f>
+        <v>1.0357142857142856</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>-8.6956521739129933E-3</v>
+      </c>
+      <c r="H16">
+        <v>16568</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>102986</v>
+      </c>
+      <c r="C17">
+        <v>96683</v>
+      </c>
+      <c r="D17">
+        <v>114</v>
+      </c>
+      <c r="E17" s="1">
+        <f>(D17/D$2)-1</f>
+        <v>1.0357142857142856</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>17060</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>104515</v>
+      </c>
+      <c r="C18">
+        <v>96842</v>
+      </c>
+      <c r="D18">
+        <v>114</v>
+      </c>
+      <c r="E18" s="1">
+        <f>(D18/D$2)-1</f>
+        <v>1.0357142857142856</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>15748</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+      <c r="F26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0AC41-34A4-4C4B-992F-CC4F79B64425}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,13 +984,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -531,399 +995,6 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>53163</v>
-      </c>
-      <c r="C2">
-        <v>55959</v>
-      </c>
-      <c r="D2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>71957</v>
-      </c>
-      <c r="C3">
-        <v>73067</v>
-      </c>
-      <c r="D3">
-        <v>76</v>
-      </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E5" si="0">(D3/D$2)-1</f>
-        <v>0.35714285714285721</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F16" si="1">(D3/D2)-1</f>
-        <v>0.35714285714285721</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>71797</v>
-      </c>
-      <c r="C4">
-        <v>72327</v>
-      </c>
-      <c r="D4">
-        <v>75</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>0.33928571428571419</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.3157894736842146E-2</v>
-      </c>
-      <c r="H4">
-        <v>16868</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>59326</v>
-      </c>
-      <c r="C5">
-        <v>69900</v>
-      </c>
-      <c r="D5">
-        <v>75</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>0.33928571428571419</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>17968</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>72364</v>
-      </c>
-      <c r="C6">
-        <v>72280</v>
-      </c>
-      <c r="D6">
-        <v>75</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" ref="E6:E14" si="2">(D6/D$2)-1</f>
-        <v>0.33928571428571419</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>17780</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>77875</v>
-      </c>
-      <c r="C7">
-        <v>76905</v>
-      </c>
-      <c r="D7">
-        <v>84</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.12000000000000011</v>
-      </c>
-      <c r="H7">
-        <v>17324</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>77435</v>
-      </c>
-      <c r="C8">
-        <v>78173</v>
-      </c>
-      <c r="D8">
-        <v>83</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="2"/>
-        <v>0.48214285714285721</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.1904761904761862E-2</v>
-      </c>
-      <c r="H8">
-        <v>16972</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>78045</v>
-      </c>
-      <c r="C9">
-        <v>69808</v>
-      </c>
-      <c r="D9">
-        <v>88</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="2"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="1"/>
-        <v>6.024096385542177E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>78585</v>
-      </c>
-      <c r="C10">
-        <v>70771</v>
-      </c>
-      <c r="D10">
-        <v>90</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="2"/>
-        <v>0.60714285714285721</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="1"/>
-        <v>2.2727272727272707E-2</v>
-      </c>
-      <c r="H10">
-        <v>16928</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>92</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="2"/>
-        <v>0.64285714285714279</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="1"/>
-        <v>2.2222222222222143E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>82020</v>
-      </c>
-      <c r="C12">
-        <v>72108</v>
-      </c>
-      <c r="D12">
-        <v>98</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="1"/>
-        <v>6.5217391304347894E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13">
-        <v>82169</v>
-      </c>
-      <c r="C13">
-        <v>73632</v>
-      </c>
-      <c r="D13">
-        <v>98</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>16908</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14">
-        <v>79126</v>
-      </c>
-      <c r="C14">
-        <v>65203</v>
-      </c>
-      <c r="D14">
-        <v>99</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="2"/>
-        <v>0.76785714285714279</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0204081632652962E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15">
-        <v>98483</v>
-      </c>
-      <c r="C15">
-        <v>90661</v>
-      </c>
-      <c r="D15">
-        <v>115</v>
-      </c>
-      <c r="E15" s="1">
-        <f>(D15/D$2)-1</f>
-        <v>1.0535714285714284</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.16161616161616155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16">
-        <v>98921</v>
-      </c>
-      <c r="C16">
-        <v>89968</v>
-      </c>
-      <c r="D16">
-        <v>114</v>
-      </c>
-      <c r="E16" s="1">
-        <f>(D16/D$2)-1</f>
-        <v>1.0357142857142856</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="1"/>
-        <v>-8.6956521739129933E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="1"/>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D27" s="1"/>
-      <c r="F27"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0AC41-34A4-4C4B-992F-CC4F79B64425}">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="B1:D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
         <v>155448</v>
       </c>
       <c r="C2">
@@ -947,11 +1018,11 @@
         <v>248</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E10" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E12" si="0">(D3/D$2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F10" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F12" si="1">(D3/D2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
     </row>
@@ -1092,6 +1163,56 @@
       <c r="F10" s="1">
         <f t="shared" si="1"/>
         <v>-2.4734982332155431E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>234741</v>
+      </c>
+      <c r="C11">
+        <v>269832</v>
+      </c>
+      <c r="D11">
+        <v>553</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.39646464646464641</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8115942028984477E-3</v>
+      </c>
+      <c r="H11">
+        <v>17060</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <v>262467</v>
+      </c>
+      <c r="C12">
+        <v>258464</v>
+      </c>
+      <c r="D12">
+        <v>555</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.4015151515151516</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6166365280290158E-3</v>
+      </c>
+      <c r="H12">
+        <v>15748</v>
       </c>
     </row>
   </sheetData>
@@ -1101,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE0C3F6-B7E9-453B-8990-B1E4EB6A41FD}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:D9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1283,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E9" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E11" si="0">(D3/D$2)-1</f>
         <v>-0.39795918367346939</v>
       </c>
       <c r="F3" s="1">
@@ -1188,7 +1309,7 @@
         <v>-0.36734693877551017</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F9" si="1">(D4/D3)-1</f>
+        <f t="shared" ref="F4:F11" si="1">(D4/D3)-1</f>
         <v>5.0847457627118731E-2</v>
       </c>
     </row>
@@ -1291,6 +1412,56 @@
       <c r="F9" s="1">
         <f t="shared" si="1"/>
         <v>-1.6393442622950838E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>64532</v>
+      </c>
+      <c r="C10">
+        <v>61035</v>
+      </c>
+      <c r="D10">
+        <v>61</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.37755102040816324</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666607E-2</v>
+      </c>
+      <c r="H10">
+        <v>18940</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>64985</v>
+      </c>
+      <c r="C11">
+        <v>63059</v>
+      </c>
+      <c r="D11">
+        <v>60</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.38775510204081631</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.6393442622950838E-2</v>
+      </c>
+      <c r="H11">
+        <v>17660</v>
       </c>
     </row>
   </sheetData>
@@ -1300,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB420C75-2FAE-4B9B-85A1-584467A6609F}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,7 +1532,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E7" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E9" si="0">(D3/D$2)-1</f>
         <v>-0.77551020408163263</v>
       </c>
       <c r="F3" s="1">
@@ -1445,6 +1616,60 @@
       <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>-0.69387755102040816</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" ref="F7:F9" si="1">(D7/D6)-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>39359</v>
+      </c>
+      <c r="C8">
+        <v>29131</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.69387755102040816</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>21616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>40498</v>
+      </c>
+      <c r="C9">
+        <v>29384</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.69387755102040816</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>20352</v>
       </c>
     </row>
   </sheetData>
@@ -1457,7 +1682,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1730,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="H2">
-        <v>16928</v>
+        <v>15748</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1544,11 +1769,11 @@
         <v>242248</v>
       </c>
       <c r="D6">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E6" s="1">
         <f>(D6/D$2)-1</f>
-        <v>3.8421052631578947</v>
+        <v>3.8508771929824563</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -1571,7 +1796,7 @@
       </c>
       <c r="F7" s="1">
         <f>(D7/D6)-1</f>
-        <v>-0.46739130434782605</v>
+        <v>-0.46835443037974689</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1585,15 +1810,15 @@
         <v>59934</v>
       </c>
       <c r="D9">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E9" s="1">
         <f>(D9/D$2)-1</f>
-        <v>-0.47368421052631582</v>
+        <v>-0.46491228070175439</v>
       </c>
       <c r="F9" s="1"/>
       <c r="H9">
-        <v>18520</v>
+        <v>17660</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1615,7 +1840,7 @@
       </c>
       <c r="F10" s="1">
         <f>(D10/D9)-1</f>
-        <v>0.23333333333333339</v>
+        <v>0.21311475409836067</v>
       </c>
       <c r="H10">
         <v>15024</v>

</xml_diff>

<commit_message>
Swap switch for if block.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E101C00F-6172-4851-8034-8130EF2619D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD3127B-E0C6-4153-BC20-0875D8CAC3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>GCC Win</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>In place sort</t>
+  </si>
+  <si>
+    <t>accept</t>
+  </si>
+  <si>
+    <t>reject</t>
+  </si>
+  <si>
+    <t>clip</t>
   </si>
 </sst>
 </file>
@@ -187,9 +196,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19275CA-BC63-49E0-893C-9314B492270F}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +583,7 @@
         <v>0.35714285714285721</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F18" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F19" si="1">(D3/D2)-1</f>
         <v>0.35714285714285721</v>
       </c>
     </row>
@@ -881,7 +891,7 @@
         <v>16568</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -906,7 +916,7 @@
         <v>17060</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -931,25 +941,107 @@
         <v>15748</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="F24"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>8.7469999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="F25"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>8.7460000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="F26"/>
+      <c r="K26">
+        <f>K24-K25</f>
+        <v>9.9999999999944578E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>305986</v>
+      </c>
+      <c r="D27" s="1">
+        <f>C27/C31</f>
+        <v>0.37616573686371607</v>
+      </c>
+      <c r="F27" s="2">
+        <v>3995</v>
+      </c>
+      <c r="G27" s="1">
+        <f>F27/F31</f>
+        <v>0.6215963902287226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28">
+        <v>498925</v>
+      </c>
+      <c r="D28" s="1">
+        <f>C28/C31</f>
+        <v>0.61335646161827506</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <f>F28/F31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29">
+        <f>813434-(C27+C28)</f>
+        <v>8523</v>
+      </c>
+      <c r="D29" s="1">
+        <f>C29/C31</f>
+        <v>1.0477801518008837E-2</v>
+      </c>
+      <c r="F29" s="2">
+        <f>6427-F27</f>
+        <v>2432</v>
+      </c>
+      <c r="G29" s="1">
+        <f>F29/F31</f>
+        <v>0.3784036097712774</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f>SUM(C27:C30)</f>
+        <v>813434</v>
+      </c>
+      <c r="F31" s="2">
+        <f>SUM(F27:F30)</f>
+        <v>6427</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Use DMA to copy vertex.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD3127B-E0C6-4153-BC20-0875D8CAC3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDF5A3E-7779-4DAA-89A4-AC66B0D3D6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="V1" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -583,7 +584,7 @@
         <v>0.35714285714285721</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F19" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F18" si="1">(D3/D2)-1</f>
         <v>0.35714285714285721</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Separate W Near clip.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDF5A3E-7779-4DAA-89A4-AC66B0D3D6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA5680C-24A5-4593-9D28-FAF4744D33E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
   <si>
     <t>GCC Win</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>clip</t>
+  </si>
+  <si>
+    <t>Separate W Clip</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +587,7 @@
         <v>0.35714285714285721</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F18" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F19" si="1">(D3/D2)-1</f>
         <v>0.35714285714285721</v>
       </c>
     </row>
@@ -940,6 +943,31 @@
       </c>
       <c r="H18">
         <v>15748</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>107261</v>
+      </c>
+      <c r="C19">
+        <v>98039</v>
+      </c>
+      <c r="D19">
+        <v>114</v>
+      </c>
+      <c r="E19" s="1">
+        <f>(D19/D$2)-1</f>
+        <v>1.0357142857142856</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>15796</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -968,8 +996,7 @@
       <c r="D26" s="1"/>
       <c r="F26"/>
       <c r="K26">
-        <f>K24-K25</f>
-        <v>9.9999999999944578E-4</v>
+        <v>8.7449999999999992</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -990,6 +1017,9 @@
         <f>F27/F31</f>
         <v>0.6215963902287226</v>
       </c>
+      <c r="K27">
+        <v>8.7420000000000009</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -1008,6 +1038,9 @@
       <c r="G28" s="1">
         <f>F28/F31</f>
         <v>0</v>
+      </c>
+      <c r="K28">
+        <v>8.74</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1052,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0AC41-34A4-4C4B-992F-CC4F79B64425}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,11 +1144,11 @@
         <v>248</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E12" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E13" si="0">(D3/D$2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F12" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F13" si="1">(D3/D2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
     </row>
@@ -1306,6 +1339,31 @@
       </c>
       <c r="H12">
         <v>15748</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>267236</v>
+      </c>
+      <c r="C13">
+        <v>265251</v>
+      </c>
+      <c r="D13">
+        <v>557</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.40656565656565657</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6036036036035668E-3</v>
+      </c>
+      <c r="H13">
+        <v>15796</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add big recip table.
Use 1/x for lerp deltas.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA5680C-24A5-4593-9D28-FAF4744D33E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA16BEC-867E-45EA-BA78-12C701AFE4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="V1" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>GCC Win</t>
   </si>
@@ -162,6 +161,30 @@
   </si>
   <si>
     <t>Separate W Clip</t>
+  </si>
+  <si>
+    <t>CRT Div</t>
+  </si>
+  <si>
+    <t>FP Div</t>
+  </si>
+  <si>
+    <t>FP Recip *</t>
+  </si>
+  <si>
+    <t>CRT recip</t>
+  </si>
+  <si>
+    <t>FP Recip</t>
+  </si>
+  <si>
+    <t>RecipTable</t>
+  </si>
+  <si>
+    <t>LerpDeltaRecip</t>
+  </si>
+  <si>
+    <t>DivRecip Lerp</t>
   </si>
 </sst>
 </file>
@@ -200,10 +223,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19275CA-BC63-49E0-893C-9314B492270F}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +611,7 @@
         <v>0.35714285714285721</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F19" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F21" si="1">(D3/D2)-1</f>
         <v>0.35714285714285721</v>
       </c>
     </row>
@@ -862,7 +886,7 @@
         <v>115</v>
       </c>
       <c r="E15" s="1">
-        <f>(D15/D$2)-1</f>
+        <f t="shared" ref="E15:E21" si="3">(D15/D$2)-1</f>
         <v>1.0535714285714284</v>
       </c>
       <c r="F15" s="1">
@@ -884,7 +908,7 @@
         <v>114</v>
       </c>
       <c r="E16" s="1">
-        <f>(D16/D$2)-1</f>
+        <f t="shared" si="3"/>
         <v>1.0357142857142856</v>
       </c>
       <c r="F16" s="1">
@@ -895,7 +919,7 @@
         <v>16568</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -909,7 +933,7 @@
         <v>114</v>
       </c>
       <c r="E17" s="1">
-        <f>(D17/D$2)-1</f>
+        <f t="shared" si="3"/>
         <v>1.0357142857142856</v>
       </c>
       <c r="F17" s="1">
@@ -920,7 +944,7 @@
         <v>17060</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -934,7 +958,7 @@
         <v>114</v>
       </c>
       <c r="E18" s="1">
-        <f>(D18/D$2)-1</f>
+        <f t="shared" si="3"/>
         <v>1.0357142857142856</v>
       </c>
       <c r="F18" s="1">
@@ -945,7 +969,7 @@
         <v>15748</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -959,7 +983,7 @@
         <v>114</v>
       </c>
       <c r="E19" s="1">
-        <f>(D19/D$2)-1</f>
+        <f t="shared" si="3"/>
         <v>1.0357142857142856</v>
       </c>
       <c r="F19" s="1">
@@ -967,39 +991,89 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>15796</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15756</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>92114</v>
+      </c>
+      <c r="C20">
+        <v>97560</v>
+      </c>
+      <c r="D20">
+        <v>116</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0714285714285716</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7543859649122862E-2</v>
+      </c>
+      <c r="H20">
+        <v>15320</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>106598</v>
+      </c>
+      <c r="C21">
+        <v>98648</v>
+      </c>
+      <c r="D21">
+        <v>116</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0714285714285716</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>15212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="F24"/>
       <c r="K24">
         <v>8.7469999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="F25"/>
       <c r="K25">
         <v>8.7460000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="F26"/>
       <c r="K26">
         <v>8.7449999999999992</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>40</v>
       </c>
@@ -1021,7 +1095,7 @@
         <v>8.7420000000000009</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -1043,7 +1117,7 @@
         <v>8.74</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -1063,11 +1137,17 @@
         <f>F29/F31</f>
         <v>0.3784036097712774</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>8.7279999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>8.5890000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C31">
         <f>SUM(C27:C30)</f>
         <v>813434</v>
@@ -1076,6 +1156,71 @@
         <f>SUM(F27:F30)</f>
         <v>6427</v>
       </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>8.6069999999999993</v>
+      </c>
+      <c r="L32">
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="3">
+        <v>124254</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="3">
+        <v>124254</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1691188</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="3">
+        <v>160926</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="3">
+        <v>77869</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="3">
+        <v>160926</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1085,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0AC41-34A4-4C4B-992F-CC4F79B64425}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,11 +1289,11 @@
         <v>248</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E13" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E15" si="0">(D3/D$2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F13" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F15" si="1">(D3/D2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
     </row>
@@ -1363,7 +1508,57 @@
         <v>3.6036036036035668E-3</v>
       </c>
       <c r="H13">
-        <v>15796</v>
+        <v>15756</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>255297</v>
+      </c>
+      <c r="C14">
+        <v>265957</v>
+      </c>
+      <c r="D14">
+        <v>556</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.40404040404040398</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.7953321364452268E-3</v>
+      </c>
+      <c r="H14">
+        <v>15320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15">
+        <v>253549</v>
+      </c>
+      <c r="C15">
+        <v>276548</v>
+      </c>
+      <c r="D15">
+        <v>549</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.38636363636363646</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.258992805755399E-2</v>
+      </c>
+      <c r="H15">
+        <v>15212</v>
       </c>
     </row>
   </sheetData>
@@ -1373,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE0C3F6-B7E9-453B-8990-B1E4EB6A41FD}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1629,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E11" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E13" si="0">(D3/D$2)-1</f>
         <v>-0.39795918367346939</v>
       </c>
       <c r="F3" s="1">
@@ -1460,7 +1655,7 @@
         <v>-0.36734693877551017</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F11" si="1">(D4/D3)-1</f>
+        <f t="shared" ref="F4:F13" si="1">(D4/D3)-1</f>
         <v>5.0847457627118731E-2</v>
       </c>
     </row>
@@ -1614,6 +1809,74 @@
       <c r="H11">
         <v>17660</v>
       </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>65316</v>
+      </c>
+      <c r="C12">
+        <v>60328</v>
+      </c>
+      <c r="D12">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.37755102040816324</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666607E-2</v>
+      </c>
+      <c r="H12">
+        <v>16920</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13">
+        <v>43176</v>
+      </c>
+      <c r="C13">
+        <v>41909</v>
+      </c>
+      <c r="D13">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.40816326530612246</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>-4.9180327868852514E-2</v>
+      </c>
+      <c r="H13">
+        <v>17012</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1622,10 +1885,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB420C75-2FAE-4B9B-85A1-584467A6609F}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1946,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E9" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E11" si="0">(D3/D$2)-1</f>
         <v>-0.77551020408163263</v>
       </c>
       <c r="F3" s="1">
@@ -1769,7 +2032,7 @@
         <v>-0.69387755102040816</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" ref="F7:F9" si="1">(D7/D6)-1</f>
+        <f t="shared" ref="F7:F11" si="1">(D7/D6)-1</f>
         <v>0</v>
       </c>
     </row>
@@ -1821,6 +2084,56 @@
       </c>
       <c r="H9">
         <v>20352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>40561</v>
+      </c>
+      <c r="C10">
+        <v>32744</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.68367346938775508</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333437E-2</v>
+      </c>
+      <c r="H10">
+        <v>19668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11">
+        <v>17938</v>
+      </c>
+      <c r="C11">
+        <v>17419</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.7857142857142857</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.32258064516129037</v>
+      </c>
+      <c r="H11">
+        <v>19568</v>
       </c>
     </row>
   </sheetData>
@@ -1833,7 +2146,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +2186,7 @@
         <v>90661</v>
       </c>
       <c r="D2">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E2" s="1">
         <f>(D2/D$2)-1</f>
@@ -1881,7 +2194,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="H2">
-        <v>15748</v>
+        <v>15212</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1899,11 +2212,11 @@
       </c>
       <c r="E3" s="1">
         <f>(D3/D$2)-1</f>
-        <v>-0.15789473684210531</v>
+        <v>-0.17241379310344829</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3" si="0">(D3/D2)-1</f>
-        <v>-0.15789473684210531</v>
+        <v>-0.17241379310344829</v>
       </c>
       <c r="H3">
         <v>15016</v>
@@ -1920,11 +2233,11 @@
         <v>242248</v>
       </c>
       <c r="D6">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="E6" s="1">
         <f>(D6/D$2)-1</f>
-        <v>3.8508771929824563</v>
+        <v>3.7327586206896548</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -1947,7 +2260,7 @@
       </c>
       <c r="F7" s="1">
         <f>(D7/D6)-1</f>
-        <v>-0.46835443037974689</v>
+        <v>-0.46448087431693985</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1961,15 +2274,15 @@
         <v>59934</v>
       </c>
       <c r="D9">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="1">
         <f>(D9/D$2)-1</f>
-        <v>-0.46491228070175439</v>
+        <v>-0.5</v>
       </c>
       <c r="F9" s="1"/>
       <c r="H9">
-        <v>17660</v>
+        <v>17012</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1991,7 +2304,7 @@
       </c>
       <c r="F10" s="1">
         <f>(D10/D9)-1</f>
-        <v>0.21311475409836067</v>
+        <v>0.27586206896551735</v>
       </c>
       <c r="H10">
         <v>15024</v>

</xml_diff>

<commit_message>
Skip subdividing polygons with low 1/w
These polygons don't shear textures very  much as they are either very small or not at large angle to camera.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA16BEC-867E-45EA-BA78-12C701AFE4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0F8D46-3F84-497E-A65E-BDAA5AC8E971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
+    <workbookView xWindow="5475" yWindow="2955" windowWidth="12090" windowHeight="11865" firstSheet="3" activeTab="4" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tex, Flags&lt;0&gt;" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>GCC Win</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>DivRecip Lerp</t>
+  </si>
+  <si>
+    <t>polys</t>
+  </si>
+  <si>
+    <t>subdivide</t>
+  </si>
+  <si>
+    <t>20% Subdivide</t>
   </si>
 </sst>
 </file>
@@ -544,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19275CA-BC63-49E0-893C-9314B492270F}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1571,7 +1580,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1638,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E13" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E14" si="0">(D3/D$2)-1</f>
         <v>-0.39795918367346939</v>
       </c>
       <c r="F3" s="1">
@@ -1655,7 +1664,7 @@
         <v>-0.36734693877551017</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F13" si="1">(D4/D3)-1</f>
+        <f t="shared" ref="F4:F14" si="1">(D4/D3)-1</f>
         <v>5.0847457627118731E-2</v>
       </c>
     </row>
@@ -1860,13 +1869,66 @@
         <v>17012</v>
       </c>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14">
+        <v>82</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.16326530612244894</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4137931034482758</v>
+      </c>
+      <c r="H14">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17">
+        <v>1480683</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18">
+        <v>335344</v>
+      </c>
+      <c r="D18">
+        <f>C18/C17</f>
+        <v>0.22647926666274956</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>14510</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3908</v>
+      </c>
+      <c r="D21">
+        <f>C21/C20</f>
+        <v>0.26933149552033081</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
@@ -2145,8 +2207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305CE264-4C44-49B5-96FC-D980F6E8E9E8}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,15 +2336,15 @@
         <v>59934</v>
       </c>
       <c r="D9">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="E9" s="1">
         <f>(D9/D$2)-1</f>
-        <v>-0.5</v>
+        <v>-0.2931034482758621</v>
       </c>
       <c r="F9" s="1"/>
       <c r="H9">
-        <v>17012</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2304,7 +2366,7 @@
       </c>
       <c r="F10" s="1">
         <f>(D10/D9)-1</f>
-        <v>0.27586206896551735</v>
+        <v>-9.7560975609756073E-2</v>
       </c>
       <c r="H10">
         <v>15024</v>

</xml_diff>

<commit_message>
Compute Z for perspective heuristic.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0F8D46-3F84-497E-A65E-BDAA5AC8E971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED3D8C6-8AB9-4940-B0AF-02865E50205F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="2955" windowWidth="12090" windowHeight="11865" firstSheet="3" activeTab="4" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tex, Flags&lt;0&gt;" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>GCC Win</t>
   </si>
@@ -151,15 +151,6 @@
     <t>In place sort</t>
   </si>
   <si>
-    <t>accept</t>
-  </si>
-  <si>
-    <t>reject</t>
-  </si>
-  <si>
-    <t>clip</t>
-  </si>
-  <si>
     <t>Separate W Clip</t>
   </si>
   <si>
@@ -194,6 +185,12 @@
   </si>
   <si>
     <t>20% Subdivide</t>
+  </si>
+  <si>
+    <t>W Near Clip Fix</t>
+  </si>
+  <si>
+    <t>25% Subdivide</t>
   </si>
 </sst>
 </file>
@@ -551,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19275CA-BC63-49E0-893C-9314B492270F}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,6 +559,7 @@
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
     <col min="5" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -572,7 +570,7 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -598,7 +596,7 @@
       <c r="C2">
         <v>55959</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>56</v>
       </c>
     </row>
@@ -612,7 +610,7 @@
       <c r="C3">
         <v>73067</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>76</v>
       </c>
       <c r="E3" s="1">
@@ -620,7 +618,7 @@
         <v>0.35714285714285721</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F21" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F22" si="1">(D3/D2)-1</f>
         <v>0.35714285714285721</v>
       </c>
     </row>
@@ -634,7 +632,7 @@
       <c r="C4">
         <v>72327</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>75</v>
       </c>
       <c r="E4" s="1">
@@ -659,7 +657,7 @@
       <c r="C5">
         <v>69900</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>75</v>
       </c>
       <c r="E5" s="1">
@@ -684,7 +682,7 @@
       <c r="C6">
         <v>72280</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>75</v>
       </c>
       <c r="E6" s="1">
@@ -709,7 +707,7 @@
       <c r="C7">
         <v>76905</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>84</v>
       </c>
       <c r="E7" s="1">
@@ -734,7 +732,7 @@
       <c r="C8">
         <v>78173</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>83</v>
       </c>
       <c r="E8" s="1">
@@ -759,7 +757,7 @@
       <c r="C9">
         <v>69808</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>88</v>
       </c>
       <c r="E9" s="1">
@@ -781,7 +779,7 @@
       <c r="C10">
         <v>70771</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>90</v>
       </c>
       <c r="E10" s="1">
@@ -800,7 +798,7 @@
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>92</v>
       </c>
       <c r="E11" s="1">
@@ -822,7 +820,7 @@
       <c r="C12">
         <v>72108</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>98</v>
       </c>
       <c r="E12" s="1">
@@ -844,7 +842,7 @@
       <c r="C13">
         <v>73632</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>98</v>
       </c>
       <c r="E13" s="1">
@@ -869,7 +867,7 @@
       <c r="C14">
         <v>65203</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>99</v>
       </c>
       <c r="E14" s="1">
@@ -891,11 +889,11 @@
       <c r="C15">
         <v>90661</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>115</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:E21" si="3">(D15/D$2)-1</f>
+        <f t="shared" ref="E15:E22" si="3">(D15/D$2)-1</f>
         <v>1.0535714285714284</v>
       </c>
       <c r="F15" s="1">
@@ -913,7 +911,7 @@
       <c r="C16">
         <v>89968</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>114</v>
       </c>
       <c r="E16" s="1">
@@ -928,7 +926,7 @@
         <v>16568</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -938,7 +936,7 @@
       <c r="C17">
         <v>96683</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>114</v>
       </c>
       <c r="E17" s="1">
@@ -953,7 +951,7 @@
         <v>17060</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -963,7 +961,7 @@
       <c r="C18">
         <v>96842</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>114</v>
       </c>
       <c r="E18" s="1">
@@ -978,9 +976,9 @@
         <v>15748</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19">
         <v>107261</v>
@@ -988,7 +986,7 @@
       <c r="C19">
         <v>98039</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>114</v>
       </c>
       <c r="E19" s="1">
@@ -1003,9 +1001,9 @@
         <v>15756</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>92114</v>
@@ -1013,7 +1011,7 @@
       <c r="C20">
         <v>97560</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>116</v>
       </c>
       <c r="E20" s="1">
@@ -1028,9 +1026,9 @@
         <v>15320</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B21">
         <v>106598</v>
@@ -1038,7 +1036,7 @@
       <c r="C21">
         <v>98648</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>116</v>
       </c>
       <c r="E21" s="1">
@@ -1053,182 +1051,129 @@
         <v>15212</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D22" s="1"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
+        <v>107388</v>
+      </c>
+      <c r="C22">
+        <v>98444</v>
+      </c>
+      <c r="D22" s="2">
+        <v>116</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0714285714285716</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>15208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D24" s="1"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E24"/>
       <c r="F24"/>
-      <c r="K24">
-        <v>8.7469999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E25"/>
       <c r="F25"/>
-      <c r="K25">
-        <v>8.7460000000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E26"/>
       <c r="F26"/>
-      <c r="K26">
-        <v>8.7449999999999992</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27">
-        <v>305986</v>
-      </c>
-      <c r="D27" s="1">
-        <f>C27/C31</f>
-        <v>0.37616573686371607</v>
-      </c>
-      <c r="F27" s="2">
-        <v>3995</v>
-      </c>
-      <c r="G27" s="1">
-        <f>F27/F31</f>
-        <v>0.6215963902287226</v>
-      </c>
-      <c r="K27">
-        <v>8.7420000000000009</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E27"/>
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E28"/>
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E29"/>
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E30"/>
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E31"/>
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E32"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E33"/>
+      <c r="F33"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>41</v>
-      </c>
-      <c r="C28">
-        <v>498925</v>
-      </c>
-      <c r="D28" s="1">
-        <f>C28/C31</f>
-        <v>0.61335646161827506</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1">
-        <f>F28/F31</f>
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>8.74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29">
-        <f>813434-(C27+C28)</f>
-        <v>8523</v>
-      </c>
-      <c r="D29" s="1">
-        <f>C29/C31</f>
-        <v>1.0477801518008837E-2</v>
-      </c>
-      <c r="F29" s="2">
-        <f>6427-F27</f>
-        <v>2432</v>
-      </c>
-      <c r="G29" s="1">
-        <f>F29/F31</f>
-        <v>0.3784036097712774</v>
-      </c>
-      <c r="K29">
-        <v>8.7279999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F30" s="2"/>
-      <c r="K30">
-        <v>8.5890000000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <f>SUM(C27:C30)</f>
-        <v>813434</v>
-      </c>
-      <c r="F31" s="2">
-        <f>SUM(F27:F30)</f>
-        <v>6427</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K32">
-        <v>8.6069999999999993</v>
-      </c>
-      <c r="L32">
-        <v>8.61</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>44</v>
       </c>
       <c r="C39" s="3">
         <v>124254</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C40" s="3">
         <v>124254</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C41" s="3">
         <v>1691188</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C44" s="3">
         <v>160926</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C45" s="3">
         <v>77869</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C46" s="3">
         <v>160926</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C47" s="3"/>
     </row>
   </sheetData>
@@ -1239,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0AC41-34A4-4C4B-992F-CC4F79B64425}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,11 +1243,11 @@
         <v>248</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E15" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E16" si="0">(D3/D$2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F15" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F16" si="1">(D3/D2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
     </row>
@@ -1497,7 +1442,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>267236</v>
@@ -1522,7 +1467,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B14">
         <v>255297</v>
@@ -1547,7 +1492,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>253549</v>
@@ -1568,6 +1513,31 @@
       </c>
       <c r="H15">
         <v>15212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <v>256016</v>
+      </c>
+      <c r="C16">
+        <v>253228</v>
+      </c>
+      <c r="D16">
+        <v>549</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.38636363636363646</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>15208</v>
       </c>
     </row>
   </sheetData>
@@ -1577,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE0C3F6-B7E9-453B-8990-B1E4EB6A41FD}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,7 +1608,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E14" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E15" si="0">(D3/D$2)-1</f>
         <v>-0.39795918367346939</v>
       </c>
       <c r="F3" s="1">
@@ -1664,7 +1634,7 @@
         <v>-0.36734693877551017</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F14" si="1">(D4/D3)-1</f>
+        <f t="shared" ref="F4:F15" si="1">(D4/D3)-1</f>
         <v>5.0847457627118731E-2</v>
       </c>
     </row>
@@ -1821,7 +1791,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>65316</v>
@@ -1846,7 +1816,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>43176</v>
@@ -1871,7 +1841,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>82</v>
@@ -1888,42 +1858,58 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17">
-        <v>1480683</v>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15">
+        <v>84</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.1428571428571429</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4390243902439046E-2</v>
+      </c>
+      <c r="H15">
+        <v>16704</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C18">
-        <v>335344</v>
-      </c>
-      <c r="D18">
-        <f>C18/C17</f>
-        <v>0.22647926666274956</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>14510</v>
+        <v>1913052</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>496734</v>
+      </c>
+      <c r="D19" s="1">
+        <f>C19/C18</f>
+        <v>0.25965525244478455</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C21">
-        <v>3908</v>
-      </c>
-      <c r="D21">
-        <f>C21/C20</f>
-        <v>0.26933149552033081</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I30" s="1"/>
+        <v>10948</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2739</v>
+      </c>
+      <c r="D22">
+        <f>C22/C21</f>
+        <v>0.25018268176835951</v>
+      </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I31" s="1"/>
@@ -1939,6 +1925,9 @@
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1947,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB420C75-2FAE-4B9B-85A1-584467A6609F}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,7 +1997,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E11" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E12" si="0">(D3/D$2)-1</f>
         <v>-0.77551020408163263</v>
       </c>
       <c r="F3" s="1">
@@ -2094,7 +2083,7 @@
         <v>-0.69387755102040816</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" ref="F7:F11" si="1">(D7/D6)-1</f>
+        <f t="shared" ref="F7:F12" si="1">(D7/D6)-1</f>
         <v>0</v>
       </c>
     </row>
@@ -2150,7 +2139,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10">
         <v>40561</v>
@@ -2175,7 +2164,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B11">
         <v>17938</v>
@@ -2196,6 +2185,31 @@
       </c>
       <c r="H11">
         <v>19568</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12">
+        <v>17909</v>
+      </c>
+      <c r="C12">
+        <v>16789</v>
+      </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.7857142857142857</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>19564</v>
       </c>
     </row>
   </sheetData>
@@ -2207,8 +2221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305CE264-4C44-49B5-96FC-D980F6E8E9E8}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,7 +2270,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="H2">
-        <v>15212</v>
+        <v>15208</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2336,15 +2350,15 @@
         <v>59934</v>
       </c>
       <c r="D9">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="1">
         <f>(D9/D$2)-1</f>
-        <v>-0.2931034482758621</v>
+        <v>-0.27586206896551724</v>
       </c>
       <c r="F9" s="1"/>
       <c r="H9">
-        <v>16384</v>
+        <v>16704</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2366,7 +2380,7 @@
       </c>
       <c r="F10" s="1">
         <f>(D10/D9)-1</f>
-        <v>-9.7560975609756073E-2</v>
+        <v>-0.11904761904761907</v>
       </c>
       <c r="H10">
         <v>15024</v>

</xml_diff>

<commit_message>
Correct fp z calculation
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED3D8C6-8AB9-4940-B0AF-02865E50205F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D073FDC0-5571-457A-8473-4DADAAF32097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tex, Flags&lt;0&gt;" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B22" sqref="B22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,7 +1187,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE0C3F6-B7E9-453B-8990-B1E4EB6A41FD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,7 +1939,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,8 +2221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305CE264-4C44-49B5-96FC-D980F6E8E9E8}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,10 +2256,10 @@
         <v>18</v>
       </c>
       <c r="B2">
-        <v>98483</v>
+        <v>107388</v>
       </c>
       <c r="C2">
-        <v>90661</v>
+        <v>98444</v>
       </c>
       <c r="D2">
         <v>116</v>
@@ -2303,10 +2303,10 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>248138</v>
+        <v>256016</v>
       </c>
       <c r="C6">
-        <v>242248</v>
+        <v>253228</v>
       </c>
       <c r="D6">
         <v>549</v>
@@ -2344,10 +2344,10 @@
         <v>27</v>
       </c>
       <c r="B9">
-        <v>62589</v>
+        <v>43176</v>
       </c>
       <c r="C9">
-        <v>59934</v>
+        <v>41909</v>
       </c>
       <c r="D9">
         <v>84</v>

</xml_diff>

<commit_message>
Remove dependency on Z for fog.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D073FDC0-5571-457A-8473-4DADAAF32097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2156D22F-6A1C-4C22-A454-769786A0D868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tex, Flags&lt;0&gt;" sheetId="1" r:id="rId1"/>
@@ -1547,15 +1547,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE0C3F6-B7E9-453B-8990-B1E4EB6A41FD}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1877,7 +1878,7 @@
         <v>16704</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>49</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>1913052</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>50</v>
       </c>
@@ -1897,12 +1898,12 @@
         <v>0.25965525244478455</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>10948</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>2739</v>
       </c>
@@ -1911,10 +1912,20 @@
         <v>0.25018268176835951</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>-25.2100830078125</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>-25.2100830078125</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
@@ -2221,7 +2232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305CE264-4C44-49B5-96FC-D980F6E8E9E8}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fog and light in Palette mode WIP.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2156D22F-6A1C-4C22-A454-769786A0D868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B7E769-768E-44BA-8038-AF04A330EC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
@@ -1184,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0AC41-34A4-4C4B-992F-CC4F79B64425}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,11 +1243,11 @@
         <v>248</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E16" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E17" si="0">(D3/D$2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F16" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F17" si="1">(D3/D2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
     </row>
@@ -1538,6 +1538,16 @@
       </c>
       <c r="H16">
         <v>15208</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -1547,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE0C3F6-B7E9-453B-8990-B1E4EB6A41FD}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,7 +1619,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E15" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E16" si="0">(D3/D$2)-1</f>
         <v>-0.39795918367346939</v>
       </c>
       <c r="F3" s="1">
@@ -1635,7 +1645,7 @@
         <v>-0.36734693877551017</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F15" si="1">(D4/D3)-1</f>
+        <f t="shared" ref="F4:F16" si="1">(D4/D3)-1</f>
         <v>5.0847457627118731E-2</v>
       </c>
     </row>
@@ -1878,67 +1888,99 @@
         <v>16704</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="C18">
+      <c r="C25">
         <v>1913052</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="C19">
+      <c r="C26">
         <v>496734</v>
       </c>
-      <c r="D19" s="1">
-        <f>C19/C18</f>
+      <c r="D26" s="1">
+        <f>C26/C25</f>
         <v>0.25965525244478455</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C21">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C28">
         <v>10948</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C22">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C29">
         <v>2739</v>
       </c>
-      <c r="D22">
-        <f>C22/C21</f>
+      <c r="D29">
+        <f>C29/C28</f>
         <v>0.25018268176835951</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L26">
+    <row r="33" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L33">
         <v>-25.2100830078125</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L27">
+    <row r="34" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L34">
         <v>-25.2100830078125</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="1"/>
+    <row r="38" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Misc tweaks and fixes.
</commit_message>
<xml_diff>
--- a/P3DBenchmark/Performance.xlsx
+++ b/P3DBenchmark/Performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\P3DBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFABBFCC-23A2-433C-9902-5B440A7A8956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E09848-82A5-4829-BA9D-9E45A9AA7494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="20415" windowHeight="15585" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{86B0D043-EEC2-43D0-BCB6-CB5E79D6E46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tex, Flags&lt;0&gt;" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="69">
   <si>
     <t>GCC Win</t>
   </si>
@@ -218,6 +218,27 @@
   </si>
   <si>
     <t>No matrix flags</t>
+  </si>
+  <si>
+    <t>GCC 15.1</t>
+  </si>
+  <si>
+    <t>Fast Fill</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>funswitch-loops</t>
+  </si>
+  <si>
+    <t>Hot Fn</t>
+  </si>
+  <si>
+    <t>No align Fn</t>
+  </si>
+  <si>
+    <t>No sched inst</t>
   </si>
 </sst>
 </file>
@@ -577,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19275CA-BC63-49E0-893C-9314B492270F}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +666,7 @@
         <v>0.35714285714285721</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F26" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F30" si="1">(D3/D2)-1</f>
         <v>0.35714285714285721</v>
       </c>
     </row>
@@ -920,7 +941,7 @@
         <v>115</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:E26" si="3">(D15/D$2)-1</f>
+        <f t="shared" ref="E15:E30" si="3">(D15/D$2)-1</f>
         <v>1.0535714285714284</v>
       </c>
       <c r="F15" s="1">
@@ -1198,20 +1219,74 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E27"/>
-      <c r="F27"/>
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="2">
+        <v>110</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>0.96428571428571419</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.5087719298245612E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E28"/>
-      <c r="F28"/>
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="2">
+        <v>117</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0892857142857144</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>6.3636363636363713E-2</v>
+      </c>
+      <c r="H28">
+        <v>17520</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E29"/>
-      <c r="F29"/>
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="2">
+        <v>110</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="3"/>
+        <v>0.96428571428571419</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>-5.9829059829059839E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E30"/>
-      <c r="F30"/>
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="2">
+        <v>115</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0535714285714284</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5454545454545414E-2</v>
+      </c>
+      <c r="H30">
+        <v>14348</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E31"/>
@@ -1290,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F0AC41-34A4-4C4B-992F-CC4F79B64425}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,11 +1424,11 @@
         <v>248</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E19" si="0">(D3/D$2)-1</f>
+        <f t="shared" ref="E3:E26" si="0">(D3/D$2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F19" si="1">(D3/D2)-1</f>
+        <f t="shared" ref="F3:F24" si="1">(D3/D2)-1</f>
         <v>-0.3737373737373737</v>
       </c>
     </row>
@@ -1710,6 +1785,125 @@
       </c>
       <c r="H19">
         <v>14192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20">
+        <v>444</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1212121212121211</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.22241681260945712</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21">
+        <v>470</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.18686868686868685</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8558558558558627E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22">
+        <v>689</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.73989898989898983</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.46595744680851059</v>
+      </c>
+      <c r="H22">
+        <v>17520</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23">
+        <v>456</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1515151515151516</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.33817126269956455</v>
+      </c>
+      <c r="H23">
+        <v>14412</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24">
+        <v>499</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26010101010101017</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4298245614035103E-2</v>
+      </c>
+      <c r="H24">
+        <v>14652</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25">
+        <v>499</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26010101010101017</v>
+      </c>
+      <c r="H25">
+        <v>14316</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26">
+        <v>499</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26010101010101017</v>
+      </c>
+      <c r="H26">
+        <v>13952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>